<commit_message>
Updated simulator choices, many restriction enzymes still present
</commit_message>
<xml_diff>
--- a/ngs_simulators.xlsx
+++ b/ngs_simulators.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-5640" yWindow="-21600" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-5720" yWindow="-21600" windowWidth="38400" windowHeight="21160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="overall_meta" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="188">
   <si>
     <t>Ref seq</t>
   </si>
@@ -591,9 +591,6 @@
     <t>Illumina and SOLiD</t>
   </si>
   <si>
-    <t>Simulator</t>
-  </si>
-  <si>
     <t>Technology</t>
   </si>
   <si>
@@ -601,6 +598,18 @@
   </si>
   <si>
     <t>Run types</t>
+  </si>
+  <si>
+    <t>in_PA</t>
+  </si>
+  <si>
+    <t>in_RE</t>
+  </si>
+  <si>
+    <t>pp_PA</t>
+  </si>
+  <si>
+    <t>out_RE</t>
   </si>
 </sst>
 </file>
@@ -744,12 +753,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1211,7 +1219,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1227,25 +1235,25 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1</v>
+        <v>185</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -1254,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>4</v>
+        <v>186</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>5</v>
@@ -1272,7 +1280,7 @@
         <v>9</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>1</v>
+        <v>187</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>10</v>
@@ -2582,10 +2590,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2595,15 +2603,15 @@
     <col min="3" max="16384" width="10.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -2611,7 +2619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -2619,7 +2627,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2627,7 +2635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -2635,7 +2643,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2643,225 +2651,181 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2917,531 +2881,531 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3645,379 +3609,379 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4054,74 +4018,74 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>